<commit_message>
Calcula dados estatísticos no ensaio da zona morta.
</commit_message>
<xml_diff>
--- a/Data/ensaio 29-06-15 (2) (cauemenegaldo)/zona_morta_01.xlsx
+++ b/Data/ensaio 29-06-15 (2) (cauemenegaldo)/zona_morta_01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
@@ -11,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Inicio de rotação (V)</t>
   </si>
@@ -33,16 +33,31 @@
     <t>Ensaio realizado em 29/06/2015 18:10
 Variando o Duty Cicle em 1% (0,012V) e anotando quando o motor inicia a rotação.</t>
   </si>
+  <si>
+    <t>média</t>
+  </si>
+  <si>
+    <t>3*std</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -200,6 +215,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -233,7 +249,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -249,9 +266,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,7 +306,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -323,7 +340,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -358,10 +374,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -534,32 +549,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="3.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="2:11" ht="30">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -569,74 +584,74 @@
       <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="2:11">
       <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="7">
         <v>5.2</v>
       </c>
       <c r="D4" s="2">
         <f>C4*0.012</f>
         <v>6.2400000000000004E-2</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="2:11">
       <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="7">
         <v>5.3</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D33" si="0">C5*0.012</f>
         <v>6.3600000000000004E-2</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" thickBot="1">
       <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="7">
         <v>6</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>7.2000000000000008E-2</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="7">
         <v>3.5</v>
       </c>
       <c r="D7" s="2">
@@ -644,11 +659,11 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="7">
         <v>5</v>
       </c>
       <c r="D8" s="2">
@@ -656,11 +671,11 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="7">
         <v>5.4</v>
       </c>
       <c r="D9" s="2">
@@ -668,11 +683,11 @@
         <v>6.480000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="7">
         <v>5</v>
       </c>
       <c r="D10" s="2">
@@ -680,11 +695,11 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="D11" s="2">
@@ -693,11 +708,11 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="7">
         <v>5</v>
       </c>
       <c r="D12" s="2">
@@ -705,11 +720,11 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11">
       <c r="B13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="D13" s="2">
@@ -717,11 +732,11 @@
         <v>5.2800000000000007E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11">
       <c r="B14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="7">
         <v>5.9</v>
       </c>
       <c r="D14" s="2">
@@ -729,11 +744,11 @@
         <v>7.0800000000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11">
       <c r="B15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="7">
         <v>4.8</v>
       </c>
       <c r="D15" s="2">
@@ -741,11 +756,11 @@
         <v>5.7599999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="7">
         <v>5.9</v>
       </c>
       <c r="D16" s="2">
@@ -753,11 +768,11 @@
         <v>7.0800000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="5">
         <v>14</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="D17" s="2">
@@ -765,11 +780,11 @@
         <v>5.2800000000000007E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="5">
         <v>15</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="7">
         <v>4.4000000000000004</v>
       </c>
       <c r="D18" s="2">
@@ -777,11 +792,11 @@
         <v>5.2800000000000007E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" s="5">
         <v>16</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="7">
         <v>4.7</v>
       </c>
       <c r="D19" s="2">
@@ -789,11 +804,11 @@
         <v>5.6400000000000006E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="5">
         <v>17</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="7">
         <v>5.4</v>
       </c>
       <c r="D20" s="2">
@@ -801,11 +816,11 @@
         <v>6.480000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="7">
         <v>5.4</v>
       </c>
       <c r="D21" s="2">
@@ -813,11 +828,11 @@
         <v>6.480000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="B22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="7">
         <v>5.7</v>
       </c>
       <c r="D22" s="2">
@@ -825,11 +840,11 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="7">
         <v>5.5</v>
       </c>
       <c r="D23" s="2">
@@ -837,11 +852,11 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" s="5">
         <v>21</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="7">
         <v>4.8</v>
       </c>
       <c r="D24" s="2">
@@ -849,11 +864,11 @@
         <v>5.7599999999999998E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4">
       <c r="B25" s="5">
         <v>22</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="7">
         <v>5.7</v>
       </c>
       <c r="D25" s="2">
@@ -861,11 +876,11 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" s="5">
         <v>23</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="7">
         <v>4.7</v>
       </c>
       <c r="D26" s="2">
@@ -873,11 +888,11 @@
         <v>5.6400000000000006E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="B27" s="5">
         <v>24</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="7">
         <v>4.7</v>
       </c>
       <c r="D27" s="2">
@@ -885,11 +900,11 @@
         <v>5.6400000000000006E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" s="5">
         <v>25</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="7">
         <v>6.2</v>
       </c>
       <c r="D28" s="2">
@@ -897,11 +912,11 @@
         <v>7.4400000000000008E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="B29" s="5">
         <v>26</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="7">
         <v>4.9000000000000004</v>
       </c>
       <c r="D29" s="2">
@@ -909,11 +924,11 @@
         <v>5.8800000000000005E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" s="5">
         <v>27</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="7">
         <v>5.3</v>
       </c>
       <c r="D30" s="2">
@@ -921,11 +936,11 @@
         <v>6.3600000000000004E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" s="5">
         <v>28</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="7">
         <v>4.2</v>
       </c>
       <c r="D31" s="2">
@@ -933,11 +948,11 @@
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="B32" s="5">
         <v>29</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="7">
         <v>6.2</v>
       </c>
       <c r="D32" s="2">
@@ -945,16 +960,54 @@
         <v>7.4400000000000008E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7">
       <c r="B33" s="5">
         <v>30</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="7">
         <v>7</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="19">
+        <f>AVERAGE(D4:D33)</f>
+        <v>6.2000000000000013E-2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="20">
+        <f>MAX(D4:D33)</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <f>STDEV(D4:D33)*3</f>
+        <v>2.6137250468803275E-2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="20">
+        <f>MIN(D4:D33)</f>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -969,24 +1022,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>